<commit_message>
found new penetration testing garbage to output
</commit_message>
<xml_diff>
--- a/Test Output Garbage Dump/HI-CRISPR Knockout/YDR210W_YOL031C_YPR030W.xlsx
+++ b/Test Output Garbage Dump/HI-CRISPR Knockout/YDR210W_YOL031C_YPR030W.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AGGTCCACCACAACAAGGTT</t>
+          <t>CGATGGTGAACTGCAACGTT</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,7 +473,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TGTTCCAACGTAACGATCCCA</t>
+          <t>ACACAAACATTTTAAACAACTGTCCA</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">

</xml_diff>

<commit_message>
lots of new test output data!
</commit_message>
<xml_diff>
--- a/Test Output Garbage Dump/HI-CRISPR Knockout/YDR210W_YOL031C_YPR030W.xlsx
+++ b/Test Output Garbage Dump/HI-CRISPR Knockout/YDR210W_YOL031C_YPR030W.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>CGATGGTGAACTGCAACGTT</t>
+          <t>CCACTCAACCATCCACTCCC</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -473,7 +473,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ACACAAACATTTTAAACAACTGTCCA</t>
+          <t>AAGGTGAGTGTGGCAAGTGG</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>GGAGGATTGTTTCTCAAGCAGC</t>
+          <t>ACCCACACACACACAACACT</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -517,7 +517,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ATGAAAGCATCGCCTGGTGA</t>
+          <t>CAGGGTAAGTGGCAGTGGAG</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -539,7 +539,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>TGATGACACCATAGAAGGAGA</t>
+          <t>TCACTCTCCAACTTCTCTGCT</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -561,7 +561,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>AGACAATTCTCCCAAACCTTGT</t>
+          <t>AGCAGATTTCGGAGGTGTGG</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">

</xml_diff>